<commit_message>
Generated response of PSSL calculation
</commit_message>
<xml_diff>
--- a/Backend/PSSL_Base_Data.xlsx
+++ b/Backend/PSSL_Base_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Portfolio" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3011" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3017" uniqueCount="279">
   <si>
     <t>Borrower</t>
   </si>
@@ -905,6 +905,21 @@
   </si>
   <si>
     <t>Applicable Collateral Value</t>
+  </si>
+  <si>
+    <t>Current Advances Outstanding</t>
+  </si>
+  <si>
+    <t>$ 271,100,000</t>
+  </si>
+  <si>
+    <t>Advances Repaid</t>
+  </si>
+  <si>
+    <t>Advances Requested</t>
+  </si>
+  <si>
+    <t>$ 0</t>
   </si>
 </sst>
 </file>
@@ -1051,7 +1066,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -1434,6 +1449,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1441,7 +1489,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1764,6 +1812,21 @@
     </xf>
     <xf numFmtId="10" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="10" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="10" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -19773,10 +19836,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19785,7 +19848,7 @@
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="82" t="s">
         <v>258</v>
       </c>
@@ -19793,7 +19856,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="83" t="s">
         <v>260</v>
       </c>
@@ -19801,7 +19864,7 @@
         <v>45716</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="83" t="s">
         <v>261</v>
       </c>
@@ -19809,7 +19872,7 @@
         <v>46413</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="83" t="s">
         <v>262</v>
       </c>
@@ -19817,7 +19880,7 @@
         <v>47144</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="83" t="s">
         <v>263</v>
       </c>
@@ -19825,7 +19888,7 @@
         <v>45716</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="83" t="s">
         <v>264</v>
       </c>
@@ -19833,7 +19896,7 @@
         <v>45736</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="83" t="s">
         <v>265</v>
       </c>
@@ -19841,19 +19904,68 @@
         <v>45716</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="83" t="s">
         <v>266</v>
       </c>
       <c r="B8" s="86"/>
     </row>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="83" t="s">
         <v>267</v>
       </c>
       <c r="B9" s="85">
         <v>45716</v>
       </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="91" t="s">
+        <v>274</v>
+      </c>
+      <c r="B11" s="94" t="s">
+        <v>275</v>
+      </c>
+      <c r="C11" s="92"/>
+      <c r="D11" s="92"/>
+      <c r="E11" s="92"/>
+      <c r="F11" s="92"/>
+      <c r="G11" s="92"/>
+      <c r="H11" s="92"/>
+      <c r="I11" s="92"/>
+      <c r="J11" s="93"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="91" t="s">
+        <v>276</v>
+      </c>
+      <c r="B12" s="95" t="s">
+        <v>278</v>
+      </c>
+      <c r="C12" s="92"/>
+      <c r="D12" s="92"/>
+      <c r="E12" s="92"/>
+      <c r="F12" s="92"/>
+      <c r="G12" s="92"/>
+      <c r="H12" s="92"/>
+      <c r="I12" s="92"/>
+      <c r="J12" s="93"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="91" t="s">
+        <v>277</v>
+      </c>
+      <c r="B13" s="95" t="s">
+        <v>278</v>
+      </c>
+      <c r="C13" s="92"/>
+      <c r="D13" s="92"/>
+      <c r="E13" s="92"/>
+      <c r="F13" s="92"/>
+      <c r="G13" s="92"/>
+      <c r="H13" s="92"/>
+      <c r="I13" s="92"/>
+      <c r="J13" s="93"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19865,7 +19977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
pssl vae data fix
</commit_message>
<xml_diff>
--- a/Backend/PSSL_Base_Data.xlsx
+++ b/Backend/PSSL_Base_Data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="107">
   <si>
     <t>Schlesinger Global, Inc.</t>
   </si>
@@ -86,9 +86,6 @@
     <t>Pequod Merger Sub Inc.</t>
   </si>
   <si>
-    <t>INVENTUS POWER, INC.</t>
-  </si>
-  <si>
     <t>LAV Gear Holdings, Inc.</t>
   </si>
   <si>
@@ -110,9 +107,6 @@
     <t>TPC US Parent, LLC</t>
   </si>
   <si>
-    <t>HW Holdco</t>
-  </si>
-  <si>
     <t>Teneo Holdings LLC</t>
   </si>
   <si>
@@ -330,6 +324,30 @@
   </si>
   <si>
     <t>$ 0</t>
+  </si>
+  <si>
+    <t>Schlesinger Global LLC</t>
+  </si>
+  <si>
+    <t>Alpine Acquisition Corp II</t>
+  </si>
+  <si>
+    <t>NORA Acquisition LLC</t>
+  </si>
+  <si>
+    <t>HW Holdco, LLC</t>
+  </si>
+  <si>
+    <t>Management Consulting &amp; Research, LLC</t>
+  </si>
+  <si>
+    <t>Urology Management Holdings, Inc</t>
+  </si>
+  <si>
+    <t>Inventus Power, Inc.</t>
+  </si>
+  <si>
+    <t>Lash Opco, LLC</t>
   </si>
 </sst>
 </file>
@@ -338,8 +356,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="169" formatCode="0.00\x"/>
-    <numFmt numFmtId="170" formatCode="&quot;₹&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="0.00\x"/>
+    <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -781,7 +799,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -814,7 +832,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="6" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -846,7 +864,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="6" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -862,7 +880,7 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="6" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -878,10 +896,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="8" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="8" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -918,10 +936,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="8" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="8" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1208,8 +1226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,54 +1247,54 @@
   <sheetData>
     <row r="1" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>48</v>
       </c>
       <c r="D2" s="10">
         <v>44217</v>
@@ -1295,13 +1313,13 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D3" s="18">
         <v>44217</v>
@@ -1323,10 +1341,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D4" s="18">
         <v>44217</v>
@@ -1345,13 +1363,13 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D5" s="18">
         <v>44217</v>
@@ -1373,10 +1391,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D6" s="18">
         <v>44217</v>
@@ -1398,10 +1416,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D7" s="18">
         <v>44217</v>
@@ -1420,13 +1438,13 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D8" s="18">
         <v>44217</v>
@@ -1448,10 +1466,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D9" s="18">
         <v>44217</v>
@@ -1480,13 +1498,13 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D10" s="18">
         <v>44255</v>
@@ -1513,13 +1531,13 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D11" s="18">
         <v>44196</v>
@@ -1546,13 +1564,13 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D12" s="18">
         <v>44255</v>
@@ -1579,13 +1597,13 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D13" s="18">
         <v>44255</v>
@@ -1612,13 +1630,13 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D14" s="18">
         <v>44371</v>
@@ -1650,10 +1668,10 @@
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D15" s="18">
         <v>44385</v>
@@ -1684,13 +1702,13 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D16" s="18">
         <v>44449</v>
@@ -1709,13 +1727,13 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="D17" s="18">
         <v>44449</v>
@@ -1747,10 +1765,10 @@
         <v>7</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D18" s="18">
         <v>44585</v>
@@ -1784,10 +1802,10 @@
         <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D19" s="18">
         <v>44585</v>
@@ -1818,13 +1836,13 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D20" s="18">
         <v>44585</v>
@@ -1855,13 +1873,13 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D21" s="18">
         <v>44609</v>
@@ -1892,13 +1910,13 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D22" s="18">
         <v>44655</v>
@@ -1929,13 +1947,13 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D23" s="18">
         <v>44655</v>
@@ -1966,13 +1984,13 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D24" s="18">
         <v>44655</v>
@@ -2006,10 +2024,10 @@
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D25" s="18">
         <v>44655</v>
@@ -2043,10 +2061,10 @@
         <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D26" s="18">
         <v>44728</v>
@@ -2077,13 +2095,13 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D27" s="18">
         <v>44718</v>
@@ -2117,10 +2135,10 @@
         <v>10</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D28" s="18">
         <v>44805</v>
@@ -2151,13 +2169,13 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D29" s="18">
         <v>44880</v>
@@ -2188,13 +2206,13 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D30" s="18">
         <v>44852</v>
@@ -2225,13 +2243,13 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D31" s="18">
         <v>44852</v>
@@ -2260,10 +2278,10 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="18">
@@ -2310,10 +2328,10 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="18">
@@ -2348,7 +2366,7 @@
         <v>11</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="18">
@@ -2383,7 +2401,7 @@
         <v>7</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="18">
@@ -2415,10 +2433,10 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="18">
@@ -2453,7 +2471,7 @@
         <v>5</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="18">
@@ -2485,13 +2503,13 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="D39" s="18">
         <v>45030</v>
@@ -2513,7 +2531,7 @@
         <v>3</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="18">
@@ -2548,7 +2566,7 @@
         <v>11</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="18">
@@ -2580,10 +2598,10 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="18">
@@ -2616,7 +2634,7 @@
         <v>9</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="18">
@@ -2651,7 +2669,7 @@
         <v>1</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="18">
@@ -2686,7 +2704,7 @@
         <v>17</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="18">
@@ -2718,10 +2736,10 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="18">
@@ -2756,7 +2774,7 @@
         <v>2</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="18">
@@ -2791,10 +2809,10 @@
         <v>10</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="D48" s="18">
         <v>45142</v>
@@ -2825,10 +2843,10 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="18">
@@ -2863,7 +2881,7 @@
         <v>8</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="18">
@@ -2893,13 +2911,13 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D51" s="18">
         <v>45216</v>
@@ -2933,7 +2951,7 @@
         <v>17</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="18">
@@ -2968,7 +2986,7 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="18">
@@ -3003,7 +3021,7 @@
         <v>11</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="18">
@@ -3053,7 +3071,7 @@
         <v>16</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="18">
@@ -3088,7 +3106,7 @@
         <v>7</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="18">
@@ -3123,10 +3141,10 @@
         <v>15</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D58" s="18">
         <v>45307</v>
@@ -3160,7 +3178,7 @@
         <v>1</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="18">
@@ -3192,10 +3210,10 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="18">
@@ -3227,10 +3245,10 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="18">
@@ -3265,10 +3283,10 @@
         <v>10</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D62" s="18">
         <v>45310</v>
@@ -3299,10 +3317,10 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="18">
@@ -3337,7 +3355,7 @@
         <v>9</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="18">
@@ -3372,10 +3390,10 @@
         <v>10</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D65" s="18">
         <v>45412</v>
@@ -3406,13 +3424,13 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D66" s="18">
         <v>45412</v>
@@ -3443,13 +3461,13 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D67" s="18">
         <v>45412</v>
@@ -3483,7 +3501,7 @@
         <v>16</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="18">
@@ -3518,7 +3536,7 @@
         <v>18</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="18">
@@ -3553,7 +3571,7 @@
         <v>13</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="18">
@@ -3588,7 +3606,7 @@
         <v>14</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="18">
@@ -3620,10 +3638,10 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="17" t="s">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="18">
@@ -3655,10 +3673,10 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="18">
@@ -3693,7 +3711,7 @@
         <v>18</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="18">
@@ -3725,10 +3743,10 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="18">
@@ -3760,10 +3778,10 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="17" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="18">
@@ -3798,10 +3816,10 @@
         <v>8</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D77" s="18">
         <v>45545</v>
@@ -3832,10 +3850,10 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="18">
@@ -3867,10 +3885,10 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="18">
@@ -3902,10 +3920,10 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="17" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="18">
@@ -3937,13 +3955,13 @@
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="17" t="s">
-        <v>17</v>
+        <v>104</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D81" s="18">
         <v>45575</v>
@@ -3974,10 +3992,10 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C82" s="1"/>
       <c r="D82" s="18">
@@ -4009,13 +4027,13 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="17" t="s">
-        <v>21</v>
+        <v>103</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D83" s="18">
         <v>45583</v>
@@ -4046,10 +4064,10 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C84" s="1"/>
       <c r="D84" s="18">
@@ -4081,10 +4099,10 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="18">
@@ -4116,10 +4134,10 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="17" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="18">
@@ -4151,13 +4169,13 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D87" s="18">
         <v>45590</v>
@@ -4188,10 +4206,10 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="17" t="s">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C88" s="1"/>
       <c r="D88" s="18">
@@ -4226,7 +4244,7 @@
         <v>2</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C89" s="1"/>
       <c r="D89" s="18">
@@ -4258,13 +4276,13 @@
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B90" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C90" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="D90" s="18">
         <v>45638</v>
@@ -4298,10 +4316,10 @@
         <v>12</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D91" s="18">
         <v>45667</v>
@@ -4332,13 +4350,13 @@
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="17" t="s">
-        <v>23</v>
+        <v>101</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D92" s="18">
         <v>45667</v>
@@ -4369,13 +4387,13 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D93" s="18">
         <v>45693</v>
@@ -4406,13 +4424,13 @@
     </row>
     <row r="94" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D94" s="27">
         <v>45708</v>
@@ -4475,15 +4493,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" s="31">
         <v>1</v>
@@ -4491,7 +4509,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B3" s="32">
         <v>1.35</v>
@@ -4499,7 +4517,7 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B4" s="32">
         <v>0.92</v>
@@ -4507,7 +4525,7 @@
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B5" s="32">
         <v>1.54</v>
@@ -4515,7 +4533,7 @@
     </row>
     <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B6" s="32">
         <v>0.79</v>
@@ -4543,15 +4561,15 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="34" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B2" s="35">
         <v>45716</v>
@@ -4559,7 +4577,7 @@
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B3" s="36">
         <v>46413</v>
@@ -4567,7 +4585,7 @@
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B4" s="36">
         <v>47144</v>
@@ -4575,7 +4593,7 @@
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B5" s="36">
         <v>45716</v>
@@ -4583,7 +4601,7 @@
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="34" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B6" s="36">
         <v>45736</v>
@@ -4591,7 +4609,7 @@
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="34" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B7" s="36">
         <v>45716</v>
@@ -4599,13 +4617,13 @@
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="34" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B8" s="37"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="34" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B9" s="36">
         <v>45716</v>
@@ -4614,10 +4632,10 @@
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="42" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B11" s="45" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C11" s="43"/>
       <c r="D11" s="43"/>
@@ -4630,10 +4648,10 @@
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="46" t="s">
         <v>98</v>
-      </c>
-      <c r="B12" s="46" t="s">
-        <v>100</v>
       </c>
       <c r="C12" s="43"/>
       <c r="D12" s="43"/>
@@ -4646,10 +4664,10 @@
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="42" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B13" s="46" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C13" s="43"/>
       <c r="D13" s="43"/>
@@ -4678,24 +4696,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="39" t="s">
         <v>93</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>94</v>
-      </c>
-      <c r="D1" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B2" s="40">
         <v>4.5</v>
@@ -4712,7 +4730,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B3" s="40">
         <v>5.5</v>
@@ -4729,7 +4747,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B4" s="40">
         <v>6.5</v>

</xml_diff>